<commit_message>
Added script for demand and throughput analysis
</commit_message>
<xml_diff>
--- a/Feasibility Analysis.xlsx
+++ b/Feasibility Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\arch-kata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91341F58-BAC0-402E-B5DD-319F4324D204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BEF20B-E04D-4FAB-B1DF-3F9E471B2B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{42D561A8-78F9-4384-9057-44562192DF9C}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{42D561A8-78F9-4384-9057-44562192DF9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Expectations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Demand</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Increased headcount</t>
   </si>
   <si>
-    <t>To meet the expected demand we would need to either increase headcount by 200%, or have 500 full-time employees</t>
-  </si>
-  <si>
     <t>Expectations / assumption</t>
   </si>
   <si>
@@ -125,6 +122,15 @@
   </si>
   <si>
     <t>Predictions</t>
+  </si>
+  <si>
+    <t>To meet the expected demand we would need to either:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - increase headcount by 200%,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - or switch to full-time employment and still extend to 500 experts.</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -348,163 +354,268 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -516,110 +627,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2882,7 +2894,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6025,7 +6036,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6036,65 +6047,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="82"/>
+      <c r="A1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1.21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>8</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>300</v>
       </c>
       <c r="I8" s="1"/>
@@ -6125,12 +6136,12 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="5" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" style="4" customWidth="1"/>
     <col min="3" max="11" width="12.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="51.42578125" style="2" customWidth="1"/>
     <col min="13" max="19" width="9.140625" style="2"/>
@@ -6139,526 +6150,517 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="9" t="s">
+      <c r="E2" s="68"/>
+      <c r="F2" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="81" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="84">
+      <c r="A3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="59">
         <v>2025</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="63">
         <v>2026</v>
       </c>
-      <c r="E3" s="87"/>
-      <c r="F3" s="86">
+      <c r="E3" s="65"/>
+      <c r="F3" s="63">
         <v>2027</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="86">
+      <c r="G3" s="64"/>
+      <c r="H3" s="63">
         <v>2028</v>
       </c>
-      <c r="I3" s="87"/>
-      <c r="J3" s="89">
+      <c r="I3" s="65"/>
+      <c r="J3" s="69">
         <v>2029</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="9"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="81"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="22" t="s">
+      <c r="A4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="81"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="13">
+      <c r="B5" s="83"/>
+      <c r="C5" s="10">
         <v>200</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <f>C5*Expectations!$B$2</f>
         <v>1000</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <f>C5*Expectations!$B$3</f>
         <v>2000</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <f>(2*D5+J5)/3</f>
         <v>1070</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <f>(2*E5+K5)/3</f>
         <v>2140</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="8">
         <f>(D5+2*J5)/3</f>
         <v>1140</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="10">
         <f>(E5+2*K5)/3</f>
         <v>2280</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <f>D5*Expectations!$B$4</f>
         <v>1210</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="10">
         <f>E5*Expectations!$B$4</f>
         <v>2420</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="82" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="39">
         <f>C5*Expectations!$B$6</f>
         <v>600</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="40">
         <f>D5*Expectations!$B$6</f>
         <v>3000</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="43">
         <f>E5*Expectations!$B$6</f>
         <v>6000</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <f t="shared" ref="F6:F8" si="0">(2*D6+J6)/3</f>
         <v>3210</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="12">
         <f t="shared" ref="G6:G8" si="1">(2*E6+K6)/3</f>
         <v>6420</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <f t="shared" ref="H6:H8" si="2">(D6+2*J6)/3</f>
         <v>3420</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <f t="shared" ref="I6:I8" si="3">(E6+2*K6)/3</f>
         <v>6840</v>
       </c>
-      <c r="J6" s="65">
+      <c r="J6" s="43">
         <f>J5*Expectations!$B$6</f>
         <v>3630</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="39">
         <f>K5*Expectations!$B$6</f>
         <v>7260</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="82"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="75"/>
+      <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="61">
+      <c r="C7" s="39">
         <f>C5*Expectations!$B$7</f>
         <v>1600</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="40">
         <f>D5*Expectations!$B$7</f>
         <v>8000</v>
       </c>
-      <c r="E7" s="65">
+      <c r="E7" s="43">
         <f>E5*Expectations!$B$7</f>
         <v>16000</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>8560</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="12">
         <f t="shared" si="1"/>
         <v>17120</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <f t="shared" si="2"/>
         <v>9120</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <f t="shared" si="3"/>
         <v>18240</v>
       </c>
-      <c r="J7" s="65">
+      <c r="J7" s="43">
         <f>J5*Expectations!$B$7</f>
         <v>9680</v>
       </c>
-      <c r="K7" s="61">
+      <c r="K7" s="39">
         <f>K5*Expectations!$B$7</f>
         <v>19360</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="82"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="36" t="s">
+      <c r="A8" s="76"/>
+      <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="41">
         <f>C6+C7</f>
         <v>2200</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="42">
         <f t="shared" ref="D8:K8" si="4">D6+D7</f>
         <v>11000</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="60">
         <f t="shared" si="4"/>
         <v>22000</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>11770</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
         <v>23540</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="14">
         <f t="shared" si="2"/>
         <v>12540</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <f t="shared" si="3"/>
         <v>25080</v>
       </c>
-      <c r="J8" s="85">
+      <c r="J8" s="60">
         <f t="shared" si="4"/>
         <v>13310</v>
       </c>
-      <c r="K8" s="63">
+      <c r="K8" s="41">
         <f t="shared" si="4"/>
         <v>26620</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="82"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="5"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="9" t="s">
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="81" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="46" t="s">
+      <c r="B29" s="78"/>
+      <c r="C29" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="21"/>
-      <c r="F29" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="9"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="81"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="89">
+      <c r="A30" s="79"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="69">
         <v>2026</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="86">
+      <c r="E30" s="70"/>
+      <c r="F30" s="63">
         <v>2027</v>
       </c>
-      <c r="G30" s="90"/>
-      <c r="H30" s="86">
+      <c r="G30" s="64"/>
+      <c r="H30" s="63">
         <v>2028</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="89">
+      <c r="I30" s="65"/>
+      <c r="J30" s="69">
         <v>2029</v>
       </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="9"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="81"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="22" t="s">
+      <c r="A31" s="79"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="23" t="s">
+      <c r="I31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K31" s="23" t="s">
+      <c r="K31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="9"/>
+      <c r="L31" s="81"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="30">
         <f>C6*Expectations!$B$5</f>
         <v>30000</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="24">
         <f>D5*Expectations!$B$5</f>
         <v>50000</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="24">
         <f>E5*Expectations!$B$5</f>
         <v>100000</v>
       </c>
-      <c r="F32" s="51">
+      <c r="F32" s="33">
         <f>F5*Expectations!$B$5</f>
         <v>53500</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="24">
         <f>G5*Expectations!$B$5</f>
         <v>107000</v>
       </c>
-      <c r="H32" s="51">
+      <c r="H32" s="33">
         <f>H5*Expectations!$B$5</f>
         <v>57000</v>
       </c>
-      <c r="I32" s="41">
+      <c r="I32" s="25">
         <f>I5*Expectations!$B$5</f>
         <v>114000</v>
       </c>
-      <c r="J32" s="40">
+      <c r="J32" s="24">
         <f>J5*Expectations!$B$5</f>
         <v>60500</v>
       </c>
-      <c r="K32" s="41">
+      <c r="K32" s="25">
         <f>K5*Expectations!$B$5</f>
         <v>121000</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="82" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29" t="s">
+      <c r="A33" s="75"/>
+      <c r="B33" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="31">
         <f>C7*Expectations!$B$5</f>
         <v>80000</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="26">
         <f>D6*Expectations!$B$5</f>
         <v>150000</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="26">
         <f>E6*Expectations!$B$5</f>
         <v>300000</v>
       </c>
-      <c r="F33" s="52">
+      <c r="F33" s="34">
         <f>F6*Expectations!$B$5</f>
         <v>160500</v>
       </c>
-      <c r="G33" s="42">
+      <c r="G33" s="26">
         <f>G6*Expectations!$B$5</f>
         <v>321000</v>
       </c>
-      <c r="H33" s="52">
+      <c r="H33" s="34">
         <f>H6*Expectations!$B$5</f>
         <v>171000</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="27">
         <f>I6*Expectations!$B$5</f>
         <v>342000</v>
       </c>
-      <c r="J33" s="42">
+      <c r="J33" s="26">
         <f>J6*Expectations!$B$5</f>
         <v>181500</v>
       </c>
-      <c r="K33" s="43">
+      <c r="K33" s="27">
         <f>K6*Expectations!$B$5</f>
         <v>363000</v>
       </c>
-      <c r="L33" s="6"/>
+      <c r="L33" s="82"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31" t="s">
+      <c r="A34" s="76"/>
+      <c r="B34" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="32">
         <f>C8*Expectations!$B$5</f>
         <v>110000</v>
       </c>
-      <c r="D34" s="44">
+      <c r="D34" s="28">
         <f>D7*Expectations!$B$5</f>
         <v>400000</v>
       </c>
-      <c r="E34" s="44">
+      <c r="E34" s="28">
         <f>E7*Expectations!$B$5</f>
         <v>800000</v>
       </c>
-      <c r="F34" s="53">
+      <c r="F34" s="35">
         <f>F7*Expectations!$B$5</f>
         <v>428000</v>
       </c>
-      <c r="G34" s="44">
+      <c r="G34" s="28">
         <f>G7*Expectations!$B$5</f>
         <v>856000</v>
       </c>
-      <c r="H34" s="53">
+      <c r="H34" s="35">
         <f>H7*Expectations!$B$5</f>
         <v>456000</v>
       </c>
-      <c r="I34" s="45">
+      <c r="I34" s="29">
         <f>I7*Expectations!$B$5</f>
         <v>912000</v>
       </c>
-      <c r="J34" s="44">
+      <c r="J34" s="28">
         <f>J7*Expectations!$B$5</f>
         <v>484000</v>
       </c>
-      <c r="K34" s="45">
+      <c r="K34" s="29">
         <f>K7*Expectations!$B$5</f>
         <v>968000</v>
       </c>
-      <c r="L34" s="6"/>
+      <c r="L34" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="A29:B31"/>
@@ -6668,9 +6670,18 @@
     <mergeCell ref="L32:L34"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6684,14 +6695,14 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="5" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" style="4" customWidth="1"/>
     <col min="3" max="7" width="15.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="2" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="2"/>
     <col min="11" max="11" width="33.5703125" style="2" customWidth="1"/>
     <col min="12" max="21" width="9.140625" style="2"/>
@@ -6700,211 +6711,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="9" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="81" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="9"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="88" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="67" t="s">
+      <c r="A3" s="86"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="9"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="68">
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="46">
         <v>1</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="36">
         <v>1.25</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="37">
         <v>1.5</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="37">
         <v>2</v>
       </c>
-      <c r="G4" s="59">
+      <c r="G4" s="38">
         <v>3</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="81"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="74">
         <v>5</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="71">
+      <c r="B5" s="83"/>
+      <c r="C5" s="47">
         <f>Expectations!$B$8*A5/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>136.36363636363637</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="48">
         <f>C5*D$4</f>
         <v>170.45454545454547</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="49">
         <f t="shared" ref="E5:G5" si="0">D5*E$4</f>
         <v>255.68181818181819</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="49">
         <f t="shared" si="0"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="50">
         <f t="shared" si="0"/>
         <v>1534.090909090909</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>25</v>
+      <c r="H5" s="92" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
         <v>8</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="75">
+      <c r="B6" s="84"/>
+      <c r="C6" s="51">
         <f>Expectations!$B$8*A6/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>218.18181818181819</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="52">
         <f t="shared" ref="D6:G9" si="1">C6*D$4</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="E6" s="77">
+      <c r="E6" s="53">
         <f t="shared" si="1"/>
         <v>409.09090909090912</v>
       </c>
-      <c r="F6" s="77">
+      <c r="F6" s="53">
         <f t="shared" si="1"/>
         <v>818.18181818181824</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="54">
         <f t="shared" si="1"/>
         <v>2454.545454545455</v>
       </c>
-      <c r="H6" s="28"/>
+      <c r="H6" s="92"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
         <v>10</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="75">
+      <c r="B7" s="84"/>
+      <c r="C7" s="51">
         <f>Expectations!$B$8*A7/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="52">
         <f t="shared" si="1"/>
         <v>340.90909090909093</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="53">
         <f t="shared" si="1"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="53">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="54">
         <f t="shared" si="1"/>
         <v>3068.181818181818</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="93" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
         <v>20</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="75">
+      <c r="B8" s="84"/>
+      <c r="C8" s="51">
         <f>Expectations!$B$8*A8/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>545.4545454545455</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="52">
         <f t="shared" si="1"/>
         <v>681.81818181818187</v>
       </c>
-      <c r="E8" s="77">
+      <c r="E8" s="53">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="53">
         <f t="shared" si="1"/>
         <v>2045.4545454545455</v>
       </c>
-      <c r="G8" s="78"/>
-      <c r="H8" s="28"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="92" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="76">
         <v>35</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="75">
+      <c r="B9" s="85"/>
+      <c r="C9" s="51">
         <f>Expectations!$B$8*A9/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>954.5454545454545</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="55">
         <f t="shared" si="1"/>
         <v>1193.181818181818</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E9" s="56">
         <f t="shared" si="1"/>
         <v>1789.772727272727</v>
       </c>
-      <c r="F9" s="80">
+      <c r="F9" s="56">
         <f t="shared" si="1"/>
         <v>3579.545454545454</v>
       </c>
-      <c r="G9" s="81"/>
-      <c r="H9" s="28"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="92"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="12">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:H4"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor updates to the feasibility sheet
</commit_message>
<xml_diff>
--- a/Feasibility Analysis.xlsx
+++ b/Feasibility Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\arch-kata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BEF20B-E04D-4FAB-B1DF-3F9E471B2B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA42CDC-FDA6-4D32-B1E5-A18853795A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{42D561A8-78F9-4384-9057-44562192DF9C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Demand</t>
   </si>
@@ -94,12 +94,6 @@
     <t>In the next 4 years we expect around 2.000 candidate applications per week, which would require over 20.000 work hours of our experts.</t>
   </si>
   <si>
-    <t>Throughtput analysis</t>
-  </si>
-  <si>
-    <t>Average availibility of an expert (hours per week)</t>
-  </si>
-  <si>
     <t>In the next 4 years we expect to spend over a million USD on the employees</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Expectations / assumption</t>
   </si>
   <si>
-    <t>Candidates processed - test 1&amp;2 (per week)</t>
-  </si>
-  <si>
     <t>Predictions</t>
   </si>
   <si>
@@ -131,6 +122,24 @@
   </si>
   <si>
     <t xml:space="preserve"> - or switch to full-time employment and still extend to 500 experts.</t>
+  </si>
+  <si>
+    <t>Throughtput analysis (per week)</t>
+  </si>
+  <si>
+    <t>Candidates processed (test 1 &amp; 2)</t>
+  </si>
+  <si>
+    <t>Expert availibility (avg.)</t>
+  </si>
+  <si>
+    <t>(current)</t>
+  </si>
+  <si>
+    <t>(half-time)</t>
+  </si>
+  <si>
+    <t>(full-time)</t>
   </si>
 </sst>
 </file>
@@ -223,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -348,13 +357,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -459,15 +505,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,9 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,87 +571,93 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,8 +670,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6047,10 +6120,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="62"/>
+      <c r="A1" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6086,7 +6159,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7">
         <v>3</v>
@@ -6094,7 +6167,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>8</v>
@@ -6103,7 +6176,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7">
         <v>300</v>
@@ -6136,7 +6209,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6150,72 +6223,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="67" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="68"/>
-      <c r="F2" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="F2" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="68"/>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="59">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="55">
         <v>2025</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="82">
         <v>2026</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63">
+      <c r="E3" s="83"/>
+      <c r="F3" s="82">
         <v>2027</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="63">
+      <c r="G3" s="84"/>
+      <c r="H3" s="82">
         <v>2028</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="69">
+      <c r="I3" s="83"/>
+      <c r="J3" s="80">
         <v>2029</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="77"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="61"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="17" t="s">
         <v>4</v>
       </c>
@@ -6240,13 +6313,13 @@
       <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="77"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="10">
         <v>200</v>
       </c>
@@ -6282,26 +6355,26 @@
         <f>E5*Expectations!$B$4</f>
         <v>2420</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="78" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="71" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="36">
         <f>C5*Expectations!$B$6</f>
         <v>600</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="37">
         <f>D5*Expectations!$B$6</f>
         <v>3000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <f>E5*Expectations!$B$6</f>
         <v>6000</v>
       </c>
@@ -6321,30 +6394,30 @@
         <f t="shared" ref="I6:I8" si="3">(E6+2*K6)/3</f>
         <v>6840</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="40">
         <f>J5*Expectations!$B$6</f>
         <v>3630</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="36">
         <f>K5*Expectations!$B$6</f>
         <v>7260</v>
       </c>
-      <c r="L6" s="82"/>
+      <c r="L6" s="78"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="36">
         <f>C5*Expectations!$B$7</f>
         <v>1600</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="37">
         <f>D5*Expectations!$B$7</f>
         <v>8000</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <f>E5*Expectations!$B$7</f>
         <v>16000</v>
       </c>
@@ -6364,30 +6437,30 @@
         <f t="shared" si="3"/>
         <v>18240</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="40">
         <f>J5*Expectations!$B$7</f>
         <v>9680</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="36">
         <f>K5*Expectations!$B$7</f>
         <v>19360</v>
       </c>
-      <c r="L7" s="82"/>
+      <c r="L7" s="78"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="38">
         <f>C6+C7</f>
         <v>2200</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="39">
         <f t="shared" ref="D8:K8" si="4">D6+D7</f>
         <v>11000</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="56">
         <f t="shared" si="4"/>
         <v>22000</v>
       </c>
@@ -6407,96 +6480,96 @@
         <f t="shared" si="3"/>
         <v>25080</v>
       </c>
-      <c r="J8" s="60">
+      <c r="J8" s="56">
         <f t="shared" si="4"/>
         <v>13310</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="38">
         <f t="shared" si="4"/>
         <v>26620</v>
       </c>
-      <c r="L8" s="82"/>
+      <c r="L8" s="78"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="81" t="s">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="71" t="s">
+      <c r="B29" s="74"/>
+      <c r="C29" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="67" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="68"/>
-      <c r="F29" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
+      <c r="F29" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
       <c r="K29" s="68"/>
-      <c r="L29" s="81"/>
+      <c r="L29" s="77"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="69">
+      <c r="A30" s="75"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="80">
         <v>2026</v>
       </c>
-      <c r="E30" s="70"/>
-      <c r="F30" s="63">
+      <c r="E30" s="81"/>
+      <c r="F30" s="82">
         <v>2027</v>
       </c>
-      <c r="G30" s="64"/>
-      <c r="H30" s="63">
+      <c r="G30" s="84"/>
+      <c r="H30" s="82">
         <v>2028</v>
       </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="69">
+      <c r="I30" s="83"/>
+      <c r="J30" s="80">
         <v>2029</v>
       </c>
-      <c r="K30" s="70"/>
-      <c r="L30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="77"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="79"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="72"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="17" t="s">
         <v>4</v>
       </c>
@@ -6521,10 +6594,10 @@
       <c r="K31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="81"/>
+      <c r="L31" s="77"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="69" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="23" t="s">
@@ -6566,12 +6639,12 @@
         <f>K5*Expectations!$B$5</f>
         <v>121000</v>
       </c>
-      <c r="L32" s="82" t="s">
-        <v>20</v>
+      <c r="L32" s="78" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="19" t="s">
         <v>8</v>
       </c>
@@ -6611,10 +6684,10 @@
         <f>K6*Expectations!$B$5</f>
         <v>363000</v>
       </c>
-      <c r="L33" s="82"/>
+      <c r="L33" s="78"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="20" t="s">
         <v>9</v>
       </c>
@@ -6654,22 +6727,15 @@
         <f>K7*Expectations!$B$5</f>
         <v>968000</v>
       </c>
-      <c r="L34" s="82"/>
+      <c r="L34" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="A29:B31"/>
     <mergeCell ref="L2:L4"/>
     <mergeCell ref="L5:L8"/>
     <mergeCell ref="L28:L31"/>
     <mergeCell ref="L32:L34"/>
     <mergeCell ref="F2:K2"/>
-    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D3:E3"/>
@@ -6681,6 +6747,13 @@
     <mergeCell ref="F29:K29"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="A29:B31"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="D29:E29"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6694,13 +6767,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8B1874-0690-4390-A2FC-E3108E5A3851}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="4" customWidth="1"/>
     <col min="3" max="7" width="15.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.7109375" style="2" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="2"/>
@@ -6711,216 +6785,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="81" t="s">
+      <c r="A1" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="77" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="81"/>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="81"/>
+      <c r="A3" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="77"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="46">
+      <c r="A4" s="94"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="95">
         <v>1</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="96">
         <v>1.25</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="97">
         <v>1.5</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="97">
         <v>2</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="98">
         <v>3</v>
       </c>
-      <c r="H4" s="81"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74">
+      <c r="A5" s="58">
         <v>5</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="47">
+      <c r="B5" s="61"/>
+      <c r="C5" s="43">
         <f>Expectations!$B$8*A5/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>136.36363636363637</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="44">
         <f>C5*D$4</f>
         <v>170.45454545454547</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="45">
         <f t="shared" ref="E5:G5" si="0">D5*E$4</f>
         <v>255.68181818181819</v>
       </c>
-      <c r="F5" s="49">
+      <c r="F5" s="45">
         <f t="shared" si="0"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="46">
         <f t="shared" si="0"/>
         <v>1534.090909090909</v>
       </c>
-      <c r="H5" s="92" t="s">
-        <v>28</v>
+      <c r="H5" s="90" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
+      <c r="A6" s="59">
         <v>8</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="51">
+      <c r="B6" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="47">
         <f>Expectations!$B$8*A6/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>218.18181818181819</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="48">
         <f t="shared" ref="D6:G9" si="1">C6*D$4</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="49">
         <f t="shared" si="1"/>
         <v>409.09090909090912</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="49">
         <f t="shared" si="1"/>
         <v>818.18181818181824</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="50">
         <f t="shared" si="1"/>
         <v>2454.545454545455</v>
       </c>
-      <c r="H6" s="92"/>
+      <c r="H6" s="90"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75">
+      <c r="A7" s="59">
         <v>10</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="51">
+      <c r="B7" s="62"/>
+      <c r="C7" s="47">
         <f>Expectations!$B$8*A7/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="48">
         <f t="shared" si="1"/>
         <v>340.90909090909093</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="49">
         <f t="shared" si="1"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="49">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="50">
         <f t="shared" si="1"/>
         <v>3068.181818181818</v>
       </c>
-      <c r="H7" s="93" t="s">
-        <v>29</v>
+      <c r="H7" s="64" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75">
+      <c r="A8" s="59">
         <v>20</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="51">
+      <c r="B8" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="47">
         <f>Expectations!$B$8*A8/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>545.4545454545455</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="48">
         <f t="shared" si="1"/>
         <v>681.81818181818187</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="49">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="49">
         <f t="shared" si="1"/>
         <v>2045.4545454545455</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="92" t="s">
-        <v>30</v>
+      <c r="G8" s="50"/>
+      <c r="H8" s="90" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76">
+      <c r="A9" s="60">
         <v>35</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="51">
+      <c r="B9" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="91">
         <f>Expectations!$B$8*A9/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>954.5454545454545</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="51">
         <f t="shared" si="1"/>
         <v>1193.181818181818</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="52">
         <f t="shared" si="1"/>
         <v>1789.772727272727</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="52">
         <f t="shared" si="1"/>
         <v>3579.545454545454</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="92"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="7">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:H4"/>
-    <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added video presentation (#24)
* Minor updates to the feasibility sheet

* Added some presentation resources

* Added gitignore

* Added presentation sound

* Finished presentation

* Add video to readme

* Cropped the video

* Minor fixes in the presentation video

---------

Co-authored-by: Paweł Wawrzynek <pawel.wawrzynek@gmail.com>
Co-authored-by: jastrza-dot <arkadiusz.jastrzebski@equiniti.com>
</commit_message>
<xml_diff>
--- a/Feasibility Analysis.xlsx
+++ b/Feasibility Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\arch-kata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BEF20B-E04D-4FAB-B1DF-3F9E471B2B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA42CDC-FDA6-4D32-B1E5-A18853795A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{42D561A8-78F9-4384-9057-44562192DF9C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Demand</t>
   </si>
@@ -94,12 +94,6 @@
     <t>In the next 4 years we expect around 2.000 candidate applications per week, which would require over 20.000 work hours of our experts.</t>
   </si>
   <si>
-    <t>Throughtput analysis</t>
-  </si>
-  <si>
-    <t>Average availibility of an expert (hours per week)</t>
-  </si>
-  <si>
     <t>In the next 4 years we expect to spend over a million USD on the employees</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Expectations / assumption</t>
   </si>
   <si>
-    <t>Candidates processed - test 1&amp;2 (per week)</t>
-  </si>
-  <si>
     <t>Predictions</t>
   </si>
   <si>
@@ -131,6 +122,24 @@
   </si>
   <si>
     <t xml:space="preserve"> - or switch to full-time employment and still extend to 500 experts.</t>
+  </si>
+  <si>
+    <t>Throughtput analysis (per week)</t>
+  </si>
+  <si>
+    <t>Candidates processed (test 1 &amp; 2)</t>
+  </si>
+  <si>
+    <t>Expert availibility (avg.)</t>
+  </si>
+  <si>
+    <t>(current)</t>
+  </si>
+  <si>
+    <t>(half-time)</t>
+  </si>
+  <si>
+    <t>(full-time)</t>
   </si>
 </sst>
 </file>
@@ -223,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -348,13 +357,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -459,15 +505,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,9 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,87 +571,93 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,8 +670,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6047,10 +6120,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="62"/>
+      <c r="A1" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6086,7 +6159,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7">
         <v>3</v>
@@ -6094,7 +6167,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>8</v>
@@ -6103,7 +6176,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7">
         <v>300</v>
@@ -6136,7 +6209,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6150,72 +6223,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="67" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="68"/>
-      <c r="F2" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="F2" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="68"/>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="59">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="55">
         <v>2025</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="82">
         <v>2026</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63">
+      <c r="E3" s="83"/>
+      <c r="F3" s="82">
         <v>2027</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="63">
+      <c r="G3" s="84"/>
+      <c r="H3" s="82">
         <v>2028</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="69">
+      <c r="I3" s="83"/>
+      <c r="J3" s="80">
         <v>2029</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="77"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="61"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="17" t="s">
         <v>4</v>
       </c>
@@ -6240,13 +6313,13 @@
       <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="77"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="10">
         <v>200</v>
       </c>
@@ -6282,26 +6355,26 @@
         <f>E5*Expectations!$B$4</f>
         <v>2420</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="78" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="71" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="36">
         <f>C5*Expectations!$B$6</f>
         <v>600</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="37">
         <f>D5*Expectations!$B$6</f>
         <v>3000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <f>E5*Expectations!$B$6</f>
         <v>6000</v>
       </c>
@@ -6321,30 +6394,30 @@
         <f t="shared" ref="I6:I8" si="3">(E6+2*K6)/3</f>
         <v>6840</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="40">
         <f>J5*Expectations!$B$6</f>
         <v>3630</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="36">
         <f>K5*Expectations!$B$6</f>
         <v>7260</v>
       </c>
-      <c r="L6" s="82"/>
+      <c r="L6" s="78"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="36">
         <f>C5*Expectations!$B$7</f>
         <v>1600</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="37">
         <f>D5*Expectations!$B$7</f>
         <v>8000</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <f>E5*Expectations!$B$7</f>
         <v>16000</v>
       </c>
@@ -6364,30 +6437,30 @@
         <f t="shared" si="3"/>
         <v>18240</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="40">
         <f>J5*Expectations!$B$7</f>
         <v>9680</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="36">
         <f>K5*Expectations!$B$7</f>
         <v>19360</v>
       </c>
-      <c r="L7" s="82"/>
+      <c r="L7" s="78"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="38">
         <f>C6+C7</f>
         <v>2200</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="39">
         <f t="shared" ref="D8:K8" si="4">D6+D7</f>
         <v>11000</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="56">
         <f t="shared" si="4"/>
         <v>22000</v>
       </c>
@@ -6407,96 +6480,96 @@
         <f t="shared" si="3"/>
         <v>25080</v>
       </c>
-      <c r="J8" s="60">
+      <c r="J8" s="56">
         <f t="shared" si="4"/>
         <v>13310</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="38">
         <f t="shared" si="4"/>
         <v>26620</v>
       </c>
-      <c r="L8" s="82"/>
+      <c r="L8" s="78"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="81" t="s">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="71" t="s">
+      <c r="B29" s="74"/>
+      <c r="C29" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="67" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="68"/>
-      <c r="F29" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
+      <c r="F29" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
       <c r="K29" s="68"/>
-      <c r="L29" s="81"/>
+      <c r="L29" s="77"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="69">
+      <c r="A30" s="75"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="80">
         <v>2026</v>
       </c>
-      <c r="E30" s="70"/>
-      <c r="F30" s="63">
+      <c r="E30" s="81"/>
+      <c r="F30" s="82">
         <v>2027</v>
       </c>
-      <c r="G30" s="64"/>
-      <c r="H30" s="63">
+      <c r="G30" s="84"/>
+      <c r="H30" s="82">
         <v>2028</v>
       </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="69">
+      <c r="I30" s="83"/>
+      <c r="J30" s="80">
         <v>2029</v>
       </c>
-      <c r="K30" s="70"/>
-      <c r="L30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="77"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="79"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="72"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="17" t="s">
         <v>4</v>
       </c>
@@ -6521,10 +6594,10 @@
       <c r="K31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="81"/>
+      <c r="L31" s="77"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="69" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="23" t="s">
@@ -6566,12 +6639,12 @@
         <f>K5*Expectations!$B$5</f>
         <v>121000</v>
       </c>
-      <c r="L32" s="82" t="s">
-        <v>20</v>
+      <c r="L32" s="78" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="19" t="s">
         <v>8</v>
       </c>
@@ -6611,10 +6684,10 @@
         <f>K6*Expectations!$B$5</f>
         <v>363000</v>
       </c>
-      <c r="L33" s="82"/>
+      <c r="L33" s="78"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="20" t="s">
         <v>9</v>
       </c>
@@ -6654,22 +6727,15 @@
         <f>K7*Expectations!$B$5</f>
         <v>968000</v>
       </c>
-      <c r="L34" s="82"/>
+      <c r="L34" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A2:B4"/>
-    <mergeCell ref="A29:B31"/>
     <mergeCell ref="L2:L4"/>
     <mergeCell ref="L5:L8"/>
     <mergeCell ref="L28:L31"/>
     <mergeCell ref="L32:L34"/>
     <mergeCell ref="F2:K2"/>
-    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D3:E3"/>
@@ -6681,6 +6747,13 @@
     <mergeCell ref="F29:K29"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="A29:B31"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="D29:E29"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6694,13 +6767,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8B1874-0690-4390-A2FC-E3108E5A3851}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="4" customWidth="1"/>
     <col min="3" max="7" width="15.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.7109375" style="2" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="2"/>
@@ -6711,216 +6785,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="81" t="s">
+      <c r="A1" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="77" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="81"/>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="81"/>
+      <c r="A3" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="77"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="46">
+      <c r="A4" s="94"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="95">
         <v>1</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="96">
         <v>1.25</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="97">
         <v>1.5</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="97">
         <v>2</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="98">
         <v>3</v>
       </c>
-      <c r="H4" s="81"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74">
+      <c r="A5" s="58">
         <v>5</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="47">
+      <c r="B5" s="61"/>
+      <c r="C5" s="43">
         <f>Expectations!$B$8*A5/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>136.36363636363637</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="44">
         <f>C5*D$4</f>
         <v>170.45454545454547</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="45">
         <f t="shared" ref="E5:G5" si="0">D5*E$4</f>
         <v>255.68181818181819</v>
       </c>
-      <c r="F5" s="49">
+      <c r="F5" s="45">
         <f t="shared" si="0"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="46">
         <f t="shared" si="0"/>
         <v>1534.090909090909</v>
       </c>
-      <c r="H5" s="92" t="s">
-        <v>28</v>
+      <c r="H5" s="90" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
+      <c r="A6" s="59">
         <v>8</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="51">
+      <c r="B6" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="47">
         <f>Expectations!$B$8*A6/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>218.18181818181819</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="48">
         <f t="shared" ref="D6:G9" si="1">C6*D$4</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="49">
         <f t="shared" si="1"/>
         <v>409.09090909090912</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="49">
         <f t="shared" si="1"/>
         <v>818.18181818181824</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="50">
         <f t="shared" si="1"/>
         <v>2454.545454545455</v>
       </c>
-      <c r="H6" s="92"/>
+      <c r="H6" s="90"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75">
+      <c r="A7" s="59">
         <v>10</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="51">
+      <c r="B7" s="62"/>
+      <c r="C7" s="47">
         <f>Expectations!$B$8*A7/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>272.72727272727275</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="48">
         <f t="shared" si="1"/>
         <v>340.90909090909093</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="49">
         <f t="shared" si="1"/>
         <v>511.36363636363637</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="49">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="50">
         <f t="shared" si="1"/>
         <v>3068.181818181818</v>
       </c>
-      <c r="H7" s="93" t="s">
-        <v>29</v>
+      <c r="H7" s="64" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75">
+      <c r="A8" s="59">
         <v>20</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="51">
+      <c r="B8" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="47">
         <f>Expectations!$B$8*A8/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>545.4545454545455</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="48">
         <f t="shared" si="1"/>
         <v>681.81818181818187</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="49">
         <f t="shared" si="1"/>
         <v>1022.7272727272727</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="49">
         <f t="shared" si="1"/>
         <v>2045.4545454545455</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="92" t="s">
-        <v>30</v>
+      <c r="G8" s="50"/>
+      <c r="H8" s="90" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76">
+      <c r="A9" s="60">
         <v>35</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="51">
+      <c r="B9" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="91">
         <f>Expectations!$B$8*A9/(Expectations!$B$6+Expectations!$B$7)</f>
         <v>954.5454545454545</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="51">
         <f t="shared" si="1"/>
         <v>1193.181818181818</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="52">
         <f t="shared" si="1"/>
         <v>1789.772727272727</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="52">
         <f t="shared" si="1"/>
         <v>3579.545454545454</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="92"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="7">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:H4"/>
-    <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>